<commit_message>
tarea 02 y nuevas preguntas
</commit_message>
<xml_diff>
--- a/preguntas/RevisionPreguntasDeExamen (3).xlsx
+++ b/preguntas/RevisionPreguntasDeExamen (3).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="17295" windowHeight="3270" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="17295" windowHeight="3270"/>
   </bookViews>
   <sheets>
     <sheet name="Examen" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="72">
   <si>
     <t>Tejero Calderera, José Vicente</t>
   </si>
@@ -269,17 +269,23 @@
     <t>a performance counte ********</t>
   </si>
   <si>
-    <t>DEBUG/TRACE ********</t>
-  </si>
-  <si>
     <t>PerformanceCounterType****</t>
+  </si>
+  <si>
+    <t>directiva de compilacion #if DEBUG</t>
+  </si>
+  <si>
+    <t>checked overflow exception</t>
+  </si>
+  <si>
+    <t>config.file log</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -305,8 +311,15 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,6 +362,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -377,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -405,6 +424,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -711,7 +733,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -721,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:AY166"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:S15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -739,12 +761,12 @@
     <row r="2" spans="1:19">
       <c r="A2">
         <f ca="1">ROUND((RAND()*17),2)</f>
-        <v>14.42</v>
+        <v>3.02</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="19">
         <v>120</v>
       </c>
       <c r="D2" s="3">
@@ -799,7 +821,7 @@
     <row r="3" spans="1:19">
       <c r="A3">
         <f t="shared" ref="A3:A16" ca="1" si="0">ROUND((RAND()*17),2)</f>
-        <v>1.07</v>
+        <v>10.68</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -859,7 +881,7 @@
     <row r="4" spans="1:19">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>12.17</v>
+        <v>14.59</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
@@ -919,7 +941,7 @@
     <row r="5" spans="1:19">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1</v>
+        <v>9.7899999999999991</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
@@ -977,7 +999,7 @@
     <row r="6" spans="1:19">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>2.33</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
@@ -1037,7 +1059,7 @@
     <row r="7" spans="1:19">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>10.93</v>
+        <v>11.91</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
@@ -1097,7 +1119,7 @@
     <row r="8" spans="1:19">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>16.649999999999999</v>
+        <v>1.99</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>6</v>
@@ -1157,7 +1179,7 @@
     <row r="9" spans="1:19">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>7.27</v>
+        <v>13.71</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>14</v>
@@ -1215,7 +1237,7 @@
     <row r="10" spans="1:19">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>13.43</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>14</v>
@@ -1273,7 +1295,7 @@
     <row r="11" spans="1:19">
       <c r="A11">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>10.87</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>15</v>
@@ -1331,7 +1353,7 @@
     <row r="12" spans="1:19">
       <c r="A12">
         <f t="shared" ca="1" si="0"/>
-        <v>16.64</v>
+        <v>1.51</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>8</v>
@@ -1389,7 +1411,7 @@
     <row r="13" spans="1:19">
       <c r="A13">
         <f t="shared" ca="1" si="0"/>
-        <v>14.59</v>
+        <v>9.48</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>9</v>
@@ -1447,7 +1469,7 @@
     <row r="14" spans="1:19">
       <c r="A14">
         <f t="shared" ca="1" si="0"/>
-        <v>11.66</v>
+        <v>10.01</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>12</v>
@@ -1507,7 +1529,7 @@
     <row r="15" spans="1:19">
       <c r="A15">
         <f t="shared" ca="1" si="0"/>
-        <v>2.48</v>
+        <v>14.95</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>10</v>
@@ -1567,7 +1589,7 @@
     <row r="16" spans="1:19">
       <c r="A16">
         <f t="shared" ca="1" si="0"/>
-        <v>16.59</v>
+        <v>16.52</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>0</v>
@@ -1590,10 +1612,10 @@
       <c r="H16" s="3">
         <v>263</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16" s="19">
         <v>86</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="19">
         <v>85</v>
       </c>
       <c r="K16" s="3">
@@ -1711,7 +1733,7 @@
       <c r="K18" s="3">
         <v>225</v>
       </c>
-      <c r="L18" s="3">
+      <c r="L18" s="19">
         <v>98</v>
       </c>
       <c r="M18" s="3">
@@ -1734,20 +1756,34 @@
       </c>
       <c r="S18" s="3">
         <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19">
+      <c r="E20">
+        <v>85</v>
+      </c>
+      <c r="F20" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="2:19">
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+      <c r="E21" s="4">
+        <v>86</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="2:19">
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+      <c r="E22" s="4">
+        <v>98</v>
+      </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -1970,8 +2006,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:S53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B51" sqref="B18:B51"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2273,8 +2309,10 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
-      <c r="A27" s="6"/>
+    <row r="27" spans="1:17" hidden="1">
+      <c r="A27" s="6">
+        <v>1</v>
+      </c>
       <c r="B27" s="12">
         <v>168</v>
       </c>
@@ -2282,13 +2320,15 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
-      <c r="A28" s="16"/>
+    <row r="28" spans="1:17" hidden="1">
+      <c r="A28" s="18">
+        <v>1</v>
+      </c>
       <c r="B28" s="12">
         <v>169</v>
       </c>
       <c r="D28" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:17" hidden="1">
@@ -2392,12 +2432,12 @@
       <c r="S37" s="3"/>
     </row>
     <row r="38" spans="1:19" ht="17.25">
-      <c r="A38" s="6"/>
+      <c r="A38" s="17"/>
       <c r="B38" s="6">
         <v>211</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:19" hidden="1">
@@ -2522,8 +2562,10 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="6"/>
+    <row r="51" spans="1:4" hidden="1">
+      <c r="A51" s="18">
+        <v>1</v>
+      </c>
       <c r="B51" s="6">
         <v>283</v>
       </c>
@@ -2534,7 +2576,7 @@
     <row r="52" spans="1:4" hidden="1">
       <c r="A52">
         <f>SUM(A2:A51)</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B52">
         <v>50</v>
@@ -2543,7 +2585,7 @@
     <row r="53" spans="1:4">
       <c r="B53">
         <f>COUNT(B2:B51)-A52</f>
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>